<commit_message>
trying to fix the relationships which i messed up
</commit_message>
<xml_diff>
--- a/y-Manipulated Tables/DataSet/Tables/STATION.xlsx
+++ b/y-Manipulated Tables/DataSet/Tables/STATION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BDSM\CSE303-sec-03-Group-03\y-Manipulated Tables\DataSet\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D320F7-09CD-4490-91C6-427BCD5484AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D886A5-6F43-418F-8339-AEA658B83579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1815" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="228">
   <si>
     <t>stationID</t>
   </si>
@@ -710,13 +710,25 @@
   </si>
   <si>
     <t>divsyl</t>
+  </si>
+  <si>
+    <t>orgID</t>
+  </si>
+  <si>
+    <t>org1</t>
+  </si>
+  <si>
+    <t>org2</t>
+  </si>
+  <si>
+    <t>org3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,6 +739,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1035,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63171248-C639-426A-8BBA-864EBEC70539}">
-  <dimension ref="A1:E209"/>
+  <dimension ref="A1:F209"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H220" sqref="H220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1067,7 @@
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1065,8 +1083,11 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f t="shared" ref="A2:A65" si="0">CONCATENATE(LEFT(D2,3),LEFT(E2,3),C2)</f>
         <v>EPAdiv1</v>
@@ -1083,8 +1104,11 @@
       <c r="E2" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv10</v>
@@ -1101,8 +1125,11 @@
       <c r="E3" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv11</v>
@@ -1119,8 +1146,11 @@
       <c r="E4" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv12</v>
@@ -1137,8 +1167,11 @@
       <c r="E5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv13</v>
@@ -1155,8 +1188,11 @@
       <c r="E6" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv16</v>
@@ -1173,8 +1209,11 @@
       <c r="E7" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv17</v>
@@ -1191,8 +1230,11 @@
       <c r="E8" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv19</v>
@@ -1209,8 +1251,11 @@
       <c r="E9" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv2</v>
@@ -1227,8 +1272,11 @@
       <c r="E10" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv20</v>
@@ -1245,8 +1293,11 @@
       <c r="E11" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv21</v>
@@ -1263,8 +1314,11 @@
       <c r="E12" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv22</v>
@@ -1281,8 +1335,11 @@
       <c r="E13" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv3</v>
@@ -1299,8 +1356,11 @@
       <c r="E14" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv4</v>
@@ -1317,8 +1377,11 @@
       <c r="E15" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv5</v>
@@ -1335,8 +1398,11 @@
       <c r="E16" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv6</v>
@@ -1353,8 +1419,11 @@
       <c r="E17" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv7</v>
@@ -1371,8 +1440,11 @@
       <c r="E18" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv9</v>
@@ -1389,8 +1461,11 @@
       <c r="E19" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv14</v>
@@ -1407,8 +1482,11 @@
       <c r="E20" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv15</v>
@@ -1425,8 +1503,11 @@
       <c r="E21" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv18</v>
@@ -1443,8 +1524,11 @@
       <c r="E22" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv23</v>
@@ -1461,8 +1545,11 @@
       <c r="E23" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv8</v>
@@ -1479,8 +1566,11 @@
       <c r="E24" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv1</v>
@@ -1497,8 +1587,11 @@
       <c r="E25" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv10</v>
@@ -1515,8 +1608,11 @@
       <c r="E26" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv11</v>
@@ -1533,8 +1629,11 @@
       <c r="E27" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv12</v>
@@ -1551,8 +1650,11 @@
       <c r="E28" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv13</v>
@@ -1569,8 +1671,11 @@
       <c r="E29" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv14</v>
@@ -1587,8 +1692,11 @@
       <c r="E30" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv15</v>
@@ -1605,8 +1713,11 @@
       <c r="E31" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv16</v>
@@ -1623,8 +1734,11 @@
       <c r="E32" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv18</v>
@@ -1641,8 +1755,11 @@
       <c r="E33" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv2</v>
@@ -1659,8 +1776,11 @@
       <c r="E34" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv20</v>
@@ -1677,8 +1797,11 @@
       <c r="E35" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv21</v>
@@ -1695,8 +1818,11 @@
       <c r="E36" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv23</v>
@@ -1713,8 +1839,11 @@
       <c r="E37" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv3</v>
@@ -1731,8 +1860,11 @@
       <c r="E38" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv4</v>
@@ -1749,8 +1881,11 @@
       <c r="E39" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv5</v>
@@ -1767,8 +1902,11 @@
       <c r="E40" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv7</v>
@@ -1785,8 +1923,11 @@
       <c r="E41" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv8</v>
@@ -1803,8 +1944,11 @@
       <c r="E42" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv9</v>
@@ -1821,8 +1965,11 @@
       <c r="E43" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv19</v>
@@ -1839,8 +1986,11 @@
       <c r="E44" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv22</v>
@@ -1857,8 +2007,11 @@
       <c r="E45" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv6</v>
@@ -1875,8 +2028,11 @@
       <c r="E46" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv17</v>
@@ -1893,8 +2049,11 @@
       <c r="E47" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv1</v>
@@ -1911,8 +2070,11 @@
       <c r="E48" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv11</v>
@@ -1929,8 +2091,11 @@
       <c r="E49" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv12</v>
@@ -1947,8 +2112,11 @@
       <c r="E50" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv13</v>
@@ -1965,8 +2133,11 @@
       <c r="E51" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv14</v>
@@ -1983,8 +2154,11 @@
       <c r="E52" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv16</v>
@@ -2001,8 +2175,11 @@
       <c r="E53" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv17</v>
@@ -2019,8 +2196,11 @@
       <c r="E54" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv18</v>
@@ -2037,8 +2217,11 @@
       <c r="E55" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv19</v>
@@ -2055,8 +2238,11 @@
       <c r="E56" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv2</v>
@@ -2073,8 +2259,11 @@
       <c r="E57" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv20</v>
@@ -2091,8 +2280,11 @@
       <c r="E58" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv21</v>
@@ -2109,8 +2301,11 @@
       <c r="E59" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv22</v>
@@ -2127,8 +2322,11 @@
       <c r="E60" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv3</v>
@@ -2145,8 +2343,11 @@
       <c r="E61" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv4</v>
@@ -2163,8 +2364,11 @@
       <c r="E62" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv6</v>
@@ -2181,8 +2385,11 @@
       <c r="E63" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv7</v>
@@ -2199,8 +2406,11 @@
       <c r="E64" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>EPAdiv8</v>
@@ -2217,8 +2427,11 @@
       <c r="E65" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" ref="A66:A129" si="1">CONCATENATE(LEFT(D66,3),LEFT(E66,3),C66)</f>
         <v>EPAdiv9</v>
@@ -2235,8 +2448,11 @@
       <c r="E66" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" si="1"/>
         <v>EPAdiv15</v>
@@ -2253,8 +2469,11 @@
       <c r="E67" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv18</v>
@@ -2271,8 +2490,11 @@
       <c r="E68" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv2</v>
@@ -2289,8 +2511,11 @@
       <c r="E69" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv20</v>
@@ -2307,8 +2532,11 @@
       <c r="E70" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv21</v>
@@ -2325,8 +2553,11 @@
       <c r="E71" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv22</v>
@@ -2343,8 +2574,11 @@
       <c r="E72" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv23</v>
@@ -2361,8 +2595,11 @@
       <c r="E73" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv3</v>
@@ -2379,8 +2616,11 @@
       <c r="E74" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv4</v>
@@ -2397,8 +2637,11 @@
       <c r="E75" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv5</v>
@@ -2415,8 +2658,11 @@
       <c r="E76" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv7</v>
@@ -2433,8 +2679,11 @@
       <c r="E77" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv8</v>
@@ -2451,8 +2700,11 @@
       <c r="E78" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv1</v>
@@ -2469,8 +2721,11 @@
       <c r="E79" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv10</v>
@@ -2487,8 +2742,11 @@
       <c r="E80" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv12</v>
@@ -2505,8 +2763,11 @@
       <c r="E81" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv13</v>
@@ -2523,8 +2784,11 @@
       <c r="E82" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv14</v>
@@ -2541,8 +2805,11 @@
       <c r="E83" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv15</v>
@@ -2559,8 +2826,11 @@
       <c r="E84" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv19</v>
@@ -2577,8 +2847,11 @@
       <c r="E85" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv6</v>
@@ -2595,8 +2868,11 @@
       <c r="E86" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv9</v>
@@ -2613,8 +2889,11 @@
       <c r="E87" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv1</v>
@@ -2631,8 +2910,11 @@
       <c r="E88" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv10</v>
@@ -2649,8 +2931,11 @@
       <c r="E89" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv11</v>
@@ -2667,8 +2952,11 @@
       <c r="E90" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv12</v>
@@ -2685,8 +2973,11 @@
       <c r="E91" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv14</v>
@@ -2703,8 +2994,11 @@
       <c r="E92" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv15</v>
@@ -2721,8 +3015,11 @@
       <c r="E93" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv16</v>
@@ -2739,8 +3036,11 @@
       <c r="E94" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F94" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv17</v>
@@ -2757,8 +3057,11 @@
       <c r="E95" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F95" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv18</v>
@@ -2775,8 +3078,11 @@
       <c r="E96" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv19</v>
@@ -2793,8 +3099,11 @@
       <c r="E97" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F97" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv2</v>
@@ -2811,8 +3120,11 @@
       <c r="E98" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv20</v>
@@ -2829,8 +3141,11 @@
       <c r="E99" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv21</v>
@@ -2847,8 +3162,11 @@
       <c r="E100" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv22</v>
@@ -2865,8 +3183,11 @@
       <c r="E101" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv23</v>
@@ -2883,8 +3204,11 @@
       <c r="E102" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F102" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv3</v>
@@ -2901,8 +3225,11 @@
       <c r="E103" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F103" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv4</v>
@@ -2919,8 +3246,11 @@
       <c r="E104" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F104" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv5</v>
@@ -2937,8 +3267,11 @@
       <c r="E105" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F105" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv6</v>
@@ -2955,8 +3288,11 @@
       <c r="E106" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F106" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv7</v>
@@ -2973,8 +3309,11 @@
       <c r="E107" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F107" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv9</v>
@@ -2991,8 +3330,11 @@
       <c r="E108" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F108" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv13</v>
@@ -3009,8 +3351,11 @@
       <c r="E109" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F109" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv8</v>
@@ -3027,8 +3372,11 @@
       <c r="E110" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F110" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv10</v>
@@ -3045,8 +3393,11 @@
       <c r="E111" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F111" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv11</v>
@@ -3063,8 +3414,11 @@
       <c r="E112" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F112" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv12</v>
@@ -3081,8 +3435,11 @@
       <c r="E113" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F113" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv13</v>
@@ -3099,8 +3456,11 @@
       <c r="E114" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F114" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv14</v>
@@ -3117,8 +3477,11 @@
       <c r="E115" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F115" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv15</v>
@@ -3135,8 +3498,11 @@
       <c r="E116" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F116" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv16</v>
@@ -3153,8 +3519,11 @@
       <c r="E117" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F117" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv17</v>
@@ -3171,8 +3540,11 @@
       <c r="E118" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F118" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv18</v>
@@ -3189,8 +3561,11 @@
       <c r="E119" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F119" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv19</v>
@@ -3207,8 +3582,11 @@
       <c r="E120" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F120" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv20</v>
@@ -3225,8 +3603,11 @@
       <c r="E121" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F121" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv21</v>
@@ -3243,8 +3624,11 @@
       <c r="E122" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F122" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv22</v>
@@ -3261,8 +3645,11 @@
       <c r="E123" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F123" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv23</v>
@@ -3279,8 +3666,11 @@
       <c r="E124" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F124" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv4</v>
@@ -3297,8 +3687,11 @@
       <c r="E125" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F125" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv5</v>
@@ -3315,8 +3708,11 @@
       <c r="E126" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F126" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv6</v>
@@ -3333,8 +3729,11 @@
       <c r="E127" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F127" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv7</v>
@@ -3351,8 +3750,11 @@
       <c r="E128" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F128" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="str">
         <f t="shared" si="1"/>
         <v>IQAdiv8</v>
@@ -3369,8 +3771,11 @@
       <c r="E129" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F129" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="str">
         <f t="shared" ref="A130:A193" si="2">CONCATENATE(LEFT(D130,3),LEFT(E130,3),C130)</f>
         <v>IQAdiv1</v>
@@ -3387,8 +3792,11 @@
       <c r="E130" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F130" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="str">
         <f t="shared" si="2"/>
         <v>IQAdiv2</v>
@@ -3405,8 +3813,11 @@
       <c r="E131" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F131" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="str">
         <f t="shared" si="2"/>
         <v>IQAdiv3</v>
@@ -3423,8 +3834,11 @@
       <c r="E132" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F132" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="str">
         <f t="shared" si="2"/>
         <v>IQAdiv9</v>
@@ -3441,8 +3855,11 @@
       <c r="E133" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F133" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="str">
         <f t="shared" si="2"/>
         <v>IQAdiv1</v>
@@ -3459,8 +3876,11 @@
       <c r="E134" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F134" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="str">
         <f t="shared" si="2"/>
         <v>IQAdiv10</v>
@@ -3477,8 +3897,11 @@
       <c r="E135" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F135" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="str">
         <f t="shared" si="2"/>
         <v>IQAdiv11</v>
@@ -3495,8 +3918,11 @@
       <c r="E136" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F136" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="str">
         <f t="shared" si="2"/>
         <v>IQAdiv12</v>
@@ -3513,8 +3939,11 @@
       <c r="E137" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F137" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="str">
         <f t="shared" si="2"/>
         <v>IQAdiv13</v>
@@ -3531,8 +3960,11 @@
       <c r="E138" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F138" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="str">
         <f t="shared" si="2"/>
         <v>IQAdiv15</v>
@@ -3549,8 +3981,11 @@
       <c r="E139" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F139" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="str">
         <f t="shared" si="2"/>
         <v>IQAdiv16</v>
@@ -3567,8 +4002,11 @@
       <c r="E140" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F140" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv18</v>
@@ -3585,8 +4023,11 @@
       <c r="E141" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F141" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv19</v>
@@ -3603,8 +4044,11 @@
       <c r="E142" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F142" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv2</v>
@@ -3621,8 +4065,11 @@
       <c r="E143" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F143" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv20</v>
@@ -3639,8 +4086,11 @@
       <c r="E144" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F144" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv21</v>
@@ -3657,8 +4107,11 @@
       <c r="E145" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F145" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv22</v>
@@ -3675,8 +4128,11 @@
       <c r="E146" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F146" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv23</v>
@@ -3693,8 +4149,11 @@
       <c r="E147" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F147" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv5</v>
@@ -3711,8 +4170,11 @@
       <c r="E148" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F148" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv6</v>
@@ -3729,8 +4191,11 @@
       <c r="E149" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F149" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv7</v>
@@ -3747,8 +4212,11 @@
       <c r="E150" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F150" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv8</v>
@@ -3765,8 +4233,11 @@
       <c r="E151" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F151" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv1</v>
@@ -3783,8 +4254,11 @@
       <c r="E152" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F152" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv11</v>
@@ -3801,8 +4275,11 @@
       <c r="E153" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F153" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv12</v>
@@ -3819,8 +4296,11 @@
       <c r="E154" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F154" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv15</v>
@@ -3837,8 +4317,11 @@
       <c r="E155" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F155" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv16</v>
@@ -3855,8 +4338,11 @@
       <c r="E156" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F156" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv17</v>
@@ -3873,8 +4359,11 @@
       <c r="E157" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F157" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv3</v>
@@ -3891,8 +4380,11 @@
       <c r="E158" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F158" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv4</v>
@@ -3909,8 +4401,11 @@
       <c r="E159" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F159" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv9</v>
@@ -3927,8 +4422,11 @@
       <c r="E160" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F160" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv10</v>
@@ -3945,8 +4443,11 @@
       <c r="E161" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F161" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv13</v>
@@ -3963,8 +4464,11 @@
       <c r="E162" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F162" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv14</v>
@@ -3981,8 +4485,11 @@
       <c r="E163" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F163" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv1</v>
@@ -3999,8 +4506,11 @@
       <c r="E164" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F164" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv10</v>
@@ -4017,8 +4527,11 @@
       <c r="E165" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F165" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv11</v>
@@ -4035,8 +4548,11 @@
       <c r="E166" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F166" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv12</v>
@@ -4053,8 +4569,11 @@
       <c r="E167" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F167" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv13</v>
@@ -4071,8 +4590,11 @@
       <c r="E168" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F168" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv14</v>
@@ -4089,8 +4611,11 @@
       <c r="E169" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F169" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv15</v>
@@ -4107,8 +4632,11 @@
       <c r="E170" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F170" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv17</v>
@@ -4125,8 +4653,11 @@
       <c r="E171" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F171" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv18</v>
@@ -4143,8 +4674,11 @@
       <c r="E172" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F172" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv19</v>
@@ -4161,8 +4695,11 @@
       <c r="E173" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F173" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv20</v>
@@ -4179,8 +4716,11 @@
       <c r="E174" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F174" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv21</v>
@@ -4197,8 +4737,11 @@
       <c r="E175" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F175" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv23</v>
@@ -4215,8 +4758,11 @@
       <c r="E176" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F176" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv3</v>
@@ -4233,8 +4779,11 @@
       <c r="E177" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F177" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv4</v>
@@ -4251,8 +4800,11 @@
       <c r="E178" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F178" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv5</v>
@@ -4269,8 +4821,11 @@
       <c r="E179" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F179" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv7</v>
@@ -4287,8 +4842,11 @@
       <c r="E180" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F180" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv16</v>
@@ -4305,8 +4863,11 @@
       <c r="E181" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F181" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv2</v>
@@ -4323,8 +4884,11 @@
       <c r="E182" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F182" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv8</v>
@@ -4341,8 +4905,11 @@
       <c r="E183" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F183" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv9</v>
@@ -4359,8 +4926,11 @@
       <c r="E184" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F184" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv22</v>
@@ -4377,8 +4947,11 @@
       <c r="E185" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F185" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv6</v>
@@ -4395,8 +4968,11 @@
       <c r="E186" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F186" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv1</v>
@@ -4413,8 +4989,11 @@
       <c r="E187" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F187" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv10</v>
@@ -4431,8 +5010,11 @@
       <c r="E188" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F188" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv11</v>
@@ -4449,8 +5031,11 @@
       <c r="E189" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F189" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv13</v>
@@ -4467,8 +5052,11 @@
       <c r="E190" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F190" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv14</v>
@@ -4485,8 +5073,11 @@
       <c r="E191" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F191" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv15</v>
@@ -4503,8 +5094,11 @@
       <c r="E192" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F192" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="str">
         <f t="shared" si="2"/>
         <v>Purdiv16</v>
@@ -4521,8 +5115,11 @@
       <c r="E193" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F193" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="str">
         <f t="shared" ref="A194:A209" si="3">CONCATENATE(LEFT(D194,3),LEFT(E194,3),C194)</f>
         <v>Purdiv17</v>
@@ -4539,8 +5136,11 @@
       <c r="E194" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F194" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="str">
         <f t="shared" si="3"/>
         <v>Purdiv18</v>
@@ -4557,8 +5157,11 @@
       <c r="E195" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F195" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="str">
         <f t="shared" si="3"/>
         <v>Purdiv19</v>
@@ -4575,8 +5178,11 @@
       <c r="E196" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F196" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="str">
         <f t="shared" si="3"/>
         <v>Purdiv2</v>
@@ -4593,8 +5199,11 @@
       <c r="E197" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F197" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="str">
         <f t="shared" si="3"/>
         <v>Purdiv20</v>
@@ -4611,8 +5220,11 @@
       <c r="E198" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F198" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="str">
         <f t="shared" si="3"/>
         <v>Purdiv21</v>
@@ -4629,8 +5241,11 @@
       <c r="E199" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F199" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="str">
         <f t="shared" si="3"/>
         <v>Purdiv23</v>
@@ -4647,8 +5262,11 @@
       <c r="E200" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F200" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="str">
         <f t="shared" si="3"/>
         <v>Purdiv3</v>
@@ -4665,8 +5283,11 @@
       <c r="E201" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F201" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="str">
         <f t="shared" si="3"/>
         <v>Purdiv5</v>
@@ -4683,8 +5304,11 @@
       <c r="E202" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F202" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="str">
         <f t="shared" si="3"/>
         <v>Purdiv7</v>
@@ -4701,8 +5325,11 @@
       <c r="E203" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F203" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="str">
         <f t="shared" si="3"/>
         <v>Purdiv8</v>
@@ -4719,8 +5346,11 @@
       <c r="E204" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F204" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="str">
         <f t="shared" si="3"/>
         <v>Purdiv12</v>
@@ -4737,8 +5367,11 @@
       <c r="E205" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F205" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="str">
         <f t="shared" si="3"/>
         <v>Purdiv22</v>
@@ -4755,8 +5388,11 @@
       <c r="E206" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F206" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="str">
         <f t="shared" si="3"/>
         <v>Purdiv4</v>
@@ -4773,8 +5409,11 @@
       <c r="E207" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F207" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="str">
         <f t="shared" si="3"/>
         <v>Purdiv6</v>
@@ -4791,8 +5430,11 @@
       <c r="E208" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F208" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="str">
         <f t="shared" si="3"/>
         <v>Purdiv9</v>
@@ -4808,6 +5450,9 @@
       </c>
       <c r="E209" t="s">
         <v>223</v>
+      </c>
+      <c r="F209" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -4815,6 +5460,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:C1034">
     <sortCondition ref="C1:C1034"/>
   </sortState>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>